<commit_message>
add stat desc, plots and readme
</commit_message>
<xml_diff>
--- a/fonction_publique/assets/codebook_base_carriere.xlsx
+++ b/fonction_publique/assets/codebook_base_carriere.xlsx
@@ -11,14 +11,13 @@
     <sheet name="etat" sheetId="2" r:id="rId2"/>
     <sheet name="qualite" sheetId="3" r:id="rId3"/>
     <sheet name="statut" sheetId="4" r:id="rId4"/>
-    <sheet name="c_netneh" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
   <si>
     <t>ident</t>
   </si>
@@ -41,12 +40,6 @@
     <t>variable</t>
   </si>
   <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
     <t>str</t>
   </si>
   <si>
@@ -243,6 +236,21 @@
   </si>
   <si>
     <t>Indice brut</t>
+  </si>
+  <si>
+    <t>categorie</t>
+  </si>
+  <si>
+    <t>int32</t>
+  </si>
+  <si>
+    <t>int16</t>
+  </si>
+  <si>
+    <t>Modifications</t>
+  </si>
+  <si>
+    <t>remplace Nan par -1</t>
   </si>
 </sst>
 </file>
@@ -791,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,173 +811,180 @@
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="168.28515625" customWidth="1"/>
+    <col min="5" max="5" width="47.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
       </c>
       <c r="D11" t="s">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="F11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E16" s="9"/>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
@@ -989,7 +1004,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1008,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D2" s="5"/>
     </row>
@@ -1017,7 +1034,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1025,7 +1042,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1033,7 +1050,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1041,7 +1058,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1049,7 +1066,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1057,7 +1074,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1065,7 +1082,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1073,7 +1090,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1081,7 +1098,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1089,7 +1106,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1097,7 +1114,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1105,7 +1122,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="5"/>
     </row>
@@ -1114,7 +1131,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1122,7 +1139,7 @@
         <v>99</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C16" s="5"/>
     </row>
@@ -1147,12 +1164,12 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1162,82 +1179,82 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1263,83 +1280,69 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>